<commit_message>
LiveRef Managesourcedata feature regression
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AAFCF2-6C04-4C5A-BA14-650E224B5E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449AF1E-A65F-4E38-B941-60072F0A9AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 3.1.0.0</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #46408</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
regression script for LIVEHTA-722 testcase
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AAFCF2-6C04-4C5A-BA14-650E224B5E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F71588-3B22-412A-B55D-B58CD70A67C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 3.1.0.0</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #47475</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
LIVEHTA-588 story regression script
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BA75AC-97AA-49E4-A79A-6B5C5FA2866A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88BC689-C3BB-4F98-B12C-C30D8FA055E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #48044</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #48445</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
LIVEHTA-1209, LIVEHTA-1084 TCs Regression scripts
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88BC689-C3BB-4F98-B12C-C30D8FA055E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DEF638-A8E5-414D-89DD-F2EC5FB37D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #48445</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49237</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Regression script for 1081, 898 and 518 stories
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DEF638-A8E5-414D-89DD-F2EC5FB37D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA18DE96-2966-480C-AA17-DAA42442E068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
+    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49237</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49753</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating the row count logic for paginations
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA18DE96-2966-480C-AA17-DAA42442E068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE3BEE8-649B-4ED9-B19B-60FB6824BE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49753</t>
+    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49950</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updating the testdata for app version check
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE3BEE8-649B-4ED9-B19B-60FB6824BE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74270B22-3461-4348-AAEC-392E360B976D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
+    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,10 @@
     <t>LiveRef</t>
   </si>
   <si>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #50015</t>
+  </si>
+  <si>
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
-  </si>
-  <si>
-    <t>Copyright @ 2022 Cytel Inc. LiveSLR 4.0.0.0 - Build #49950</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added LIVEHTA-883 TCs. Updated LiveRef reg C29826
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74270B22-3461-4348-AAEC-392E360B976D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A1717C-A241-4D56-B534-C158D9A8663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,10 @@
     <t>LiveRef</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #50015</t>
-  </si>
-  <si>
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
+  </si>
+  <si>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #51133</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the test data
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A1717C-A241-4D56-B534-C158D9A8663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45049CA0-4E5E-4FC8-B26C-1ED409F4335C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #51133</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #51276</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adding LIVEHTA-723 and LIVEHTA-931 TCs
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A57A5A-576E-4FDB-8BBF-7402ED1FB690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDB98F7-AEA0-42F9-97AC-B14C1B852D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #51921</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52677</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
Update the expected liveslr application version
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDB98F7-AEA0-42F9-97AC-B14C1B852D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0851E157-82D2-4ED6-9C7F-B91EB5C4BB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52677</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52777</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated the doc string
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0851E157-82D2-4ED6-9C7F-B91EB5C4BB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B88E97-68A0-45D2-A00A-EE3F38191AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52777</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52885</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Enhancing word report comparison with expected res
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B88E97-68A0-45D2-A00A-EE3F38191AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DC530F-3FAA-4785-82CC-21FCC6FFE0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #52885</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #53020</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
pushing env variable changes and LIVEHTA615 TCs
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DC530F-3FAA-4785-82CC-21FCC6FFE0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999AD48-7AC5-41D8-AD08-D33797554D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #53020</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #54269</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updating changes related to env setup
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999AD48-7AC5-41D8-AD08-D33797554D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB86E64-87FC-40EB-9275-D54AD1B007AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #54269</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #54694</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
Adding PICOS page validation scenario
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB86E64-87FC-40EB-9275-D54AD1B007AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C0FA7-4C4F-40F1-9927-F1F0C90E0CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #54694</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #55640</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Rectifying headless mode issue and report enhance
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C0FA7-4C4F-40F1-9927-F1F0C90E0CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF59D137-1F79-4ABE-9AA3-04D87B193F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #55640</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #57755</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated the test data and OR file
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF59D137-1F79-4ABE-9AA3-04D87B193F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07766124-1511-42DB-B198-25C0E8627E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #57755</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #58503</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
NonOnco Import tool, LIVEHTA-1328, LIVEHTA-1449
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07766124-1511-42DB-B198-25C0E8627E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AA6B0-164E-4243-82A0-693D4C4D03DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #58503</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #59654</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Resolving the linting issues
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AA6B0-164E-4243-82A0-693D4C4D03DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFC72F3-3E94-44CA-900E-27C9054961D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #59654</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #59729</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Non-Oncology latest template changes
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D55B1CC-A558-4ACD-B35E-0478610CE904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F18EA79-290E-4077-8EB8-3C2931491A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #60508</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #62050</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updating the staging testdata
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F18EA79-290E-4077-8EB8-3C2931491A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2AC2D8-58CD-43EA-9A6F-B92CC1322BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #62050</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #62134</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Test data udpate for 4.0 release
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCEF7C5-454D-428D-B84A-5FCAF1B5CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE2F0F8-146A-4E63-B0EA-ABFB4B442F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #62347</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.0.0.0 - Build #62821</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Non-Oncology import tool scenarios
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D21649-330B-487A-A4FA-6FEBF46B9DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653DA3F9-5283-4ABC-A5C5-300D5F91B783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #63989</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #64167</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updating the application version
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653DA3F9-5283-4ABC-A5C5-300D5F91B783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98343AF7-A944-4367-A49C-ED6263DC9088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #64167</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #64541</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Optimiszing and Testdata update
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDBBF44-623A-4FB7-9CE9-88A92414B1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F451B61-0C26-461B-A65B-5534D1969CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #66233</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #67334</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Non-Oncology Excel reports comparison
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943D4E97-5BA3-4967-9C64-404E2A1F831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6A07B-A4A3-4638-A9B9-8577E86C5C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #67763</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #68318</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Non-Onco scenarios for LIVEHTA-2156, LIVEHTA-2136, LIVEHTA-1960, LIVEHTA-1959, LIVEHTA-1501
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6A07B-A4A3-4638-A9B9-8577E86C5C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E1533E-59CC-4AF4-9E68-11261B018885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #68318</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #68882</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Staging env Test data update
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E1533E-59CC-4AF4-9E68-11261B018885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA704CD9-2512-451B-AF00-C2AD677E97CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #68882</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #69776</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Reg TCs for LIVEHTA-1826,  LIVEHTA-2088 and LIVEHTA-1498
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DED59-1F6C-4105-ADD9-3FFE4EAA1D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D42439-A53D-4195-9D02-DF34AD73ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #70158</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #70986</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added reuseable method for dropdown selection
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DED59-1F6C-4105-ADD9-3FFE4EAA1D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECD8870-E45A-4280-95C4-B22490BDF07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.1.0.0 - Build #70158</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #71567</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Testdata correction due to LIVEHTA-2596 and LIVEHTA-2980
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8F1C97-7783-4351-9B4D-BCEA26DA7C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3702B04F-E555-4498-9F9E-2A234A871294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #72274</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #72539</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Non-Onco Study Design functionality
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3702B04F-E555-4498-9F9E-2A234A871294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C5D21-9646-45E3-B19D-B8D3EA0B80E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #72539</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #73167</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Download Protocol reg TC
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122E600F-AFD5-42F7-A541-509E90C0820D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3517672B-E5DA-49A7-B397-5E6B462C0900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #73277</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74014</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Regression TC for story 1820
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3517672B-E5DA-49A7-B397-5E6B462C0900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52BCAFD-77D4-45F6-AE7A-1ED480EF43CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74014</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74238</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Regression tc for 1904
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52BCAFD-77D4-45F6-AE7A-1ED480EF43CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD57FE2-1F80-4915-B401-C087B0CEEFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.1.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74238</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74304</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updating the staging env testdata
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB25A395-94E5-4AF9-9C91-80D62DDDC0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C1A073-C111-4604-AB96-188E4436CEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.2.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74514</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74997</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
3004 epic regression cases
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C1A073-C111-4604-AB96-188E4436CEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D519A0C-07DE-40CB-87C4-93D899A63FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.2.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 4.2.0.0 - Build #74997</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 5.1.0.0 - Build #76045</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated pdf conversion step
</commit_message>
<xml_diff>
--- a/Testdata/Application_version_data.xlsx
+++ b/Testdata/Application_version_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19143F7-12FE-457B-BD8E-9068A1DF5124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C2C9C-81F5-4726-B8A3-73ABBF4D47ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{578ADB0F-A7B8-4894-B237-CFBBD4B1838D}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Copyright @ 2022 Cytel Inc. LiveRef™ 1.2.0.0</t>
   </si>
   <si>
-    <t>Copyright @ 2023 Cytel Inc. LiveSLR 5.1.0.0 - Build #76518</t>
+    <t>Copyright @ 2023 Cytel Inc. LiveSLR 5.1.0.0 - Build #76695</t>
   </si>
 </sst>
 </file>

</xml_diff>